<commit_message>
Updating parts list with cheaper components
</commit_message>
<xml_diff>
--- a/LPC Dev Board.xlsx
+++ b/LPC Dev Board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="169">
   <si>
     <t>Designator</t>
   </si>
@@ -453,13 +453,91 @@
   </si>
   <si>
     <t>Texas Instruments TPS7A4501DCQR</t>
+  </si>
+  <si>
+    <t>150060GS75000 are $0.34</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">better choice </t>
+  </si>
+  <si>
+    <t>865080640004 for $0.29</t>
+  </si>
+  <si>
+    <t>LPC has hysterious, this is not needed</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Replace with $12</t>
+  </si>
+  <si>
+    <t>Replace with simple pin</t>
+  </si>
+  <si>
+    <t>20021111-00010T4LF for $0.96</t>
+  </si>
+  <si>
+    <t>Replace with $8</t>
+  </si>
+  <si>
+    <t>D- D+</t>
+  </si>
+  <si>
+    <t>C0603C180J5GACTU for $0.04</t>
+  </si>
+  <si>
+    <t>CL10C200JB8NNNC for $0.04</t>
+  </si>
+  <si>
+    <t>C0603C470J1GACTU for $0.06</t>
+  </si>
+  <si>
+    <t>from 0805 to 0603 Crystal</t>
+  </si>
+  <si>
+    <t>from 0805 to 0603 D- D+</t>
+  </si>
+  <si>
+    <t>GRM188R71C104KA01D for $0.012</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ472V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ513V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ270V</t>
+  </si>
+  <si>
+    <t>Replace with $21</t>
+  </si>
+  <si>
+    <t>Replace with $26</t>
+  </si>
+  <si>
+    <t>Replace with 249k</t>
+  </si>
+  <si>
+    <t>PTS645SM43SMTR92 LFS for $0.23</t>
+  </si>
+  <si>
+    <t>Unkown bounce time, assumed 30ms</t>
+  </si>
+  <si>
+    <t>For LNR sense</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +557,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -494,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -517,11 +603,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,8 +638,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,9 +974,10 @@
     <col min="3" max="3" width="6.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.77734375" customWidth="1"/>
     <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,8 +993,17 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -893,543 +1019,634 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>1.67</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D8" s="3">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="G8" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="G9" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="G13" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="H14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D16" s="3">
         <v>11</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="F16">
+        <v>0.61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D17" s="3">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="3">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5017</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="3">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="3">
-        <v>16</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="3">
-        <v>13</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="3">
-        <v>11</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="H25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="H26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="H28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>5017</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="D34" s="3">
         <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,7 +1701,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G12" r:id="rId1" display="http://www.digikey.ca/product-detail/en/wurth-electronics-inc/865080640004/732-8449-6-ND/5729752"/>
+    <hyperlink ref="G4" r:id="rId2" display="http://www.digikey.ca/product-detail/en/amphenol-fci/20021111-00010T4LF/609-3712-ND/2209072"/>
+    <hyperlink ref="G9" r:id="rId3" display="http://www.digikey.ca/product-detail/en/kemet/C0603C180J5GACTU/399-1052-1-ND/411327"/>
+    <hyperlink ref="G10" r:id="rId4" display="http://www.digikey.ca/product-detail/en/samsung-electro-mechanics-america-inc/CL10C200JB8NNNC/1276-1187-1-ND/3889273"/>
+    <hyperlink ref="G13" r:id="rId5" display="http://www.digikey.ca/product-detail/en/kemet/C0603C470J1GACTU/399-7917-1-ND/3471640"/>
+    <hyperlink ref="G8" r:id="rId6" display="http://www.digikey.ca/product-detail/en/murata-electronics-north-america/GRM188R71C104KA01D/490-1532-1-ND/587771"/>
+    <hyperlink ref="G21" r:id="rId7" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ472V/P4.7KGCT-ND/135199"/>
+    <hyperlink ref="G22" r:id="rId8" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ513V/P51KGCT-ND/134811"/>
+    <hyperlink ref="G27" r:id="rId9" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ270V/P27GCT-ND/134668"/>
+    <hyperlink ref="G2" r:id="rId10" display="http://www.digikey.ca/product-detail/en/c-k-components/PTS645SM43SMTR92-LFS/CKN9112CT-ND/1146934"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
brought component costs down by 33% (0.00)
</commit_message>
<xml_diff>
--- a/LPC Dev Board.xlsx
+++ b/LPC Dev Board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="175">
   <si>
     <t>Designator</t>
   </si>
@@ -531,6 +531,24 @@
   </si>
   <si>
     <t>For LNR sense</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF2493V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEY0R00V</t>
+  </si>
+  <si>
+    <t>F980J107MMAAXE</t>
+  </si>
+  <si>
+    <t>100uF, gives ~30 seconds to RTC</t>
+  </si>
+  <si>
+    <t>DA2J10100L</t>
+  </si>
+  <si>
+    <t>SD card</t>
   </si>
 </sst>
 </file>
@@ -964,7 +982,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,6 +1224,12 @@
       <c r="F11">
         <v>3.12</v>
       </c>
+      <c r="G11" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1290,7 +1314,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -1329,6 +1353,9 @@
       <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="G17" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1380,6 +1407,9 @@
       <c r="E20" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="G20" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -1497,6 +1527,9 @@
       <c r="E26" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="G26" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="H26" t="s">
         <v>165</v>
       </c>
@@ -1615,7 +1648,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1632,7 +1665,7 @@
         <v>5017</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1648,8 +1681,14 @@
       <c r="E34" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G34" s="7">
+        <v>1051620101</v>
+      </c>
+      <c r="H34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
@@ -1666,7 +1705,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>117</v>
       </c>
@@ -1683,7 +1722,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>120</v>
       </c>
@@ -1712,8 +1751,13 @@
     <hyperlink ref="G22" r:id="rId8" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ513V/P51KGCT-ND/134811"/>
     <hyperlink ref="G27" r:id="rId9" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ270V/P27GCT-ND/134668"/>
     <hyperlink ref="G2" r:id="rId10" display="http://www.digikey.ca/product-detail/en/c-k-components/PTS645SM43SMTR92-LFS/CKN9112CT-ND/1146934"/>
+    <hyperlink ref="G26" r:id="rId11" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3EKF2493V/P249KHCT-ND/198275"/>
+    <hyperlink ref="G20" r:id="rId12" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3GEY0R00V/P0.0GCT-ND/134711"/>
+    <hyperlink ref="G11" r:id="rId13" display="https://www.digikey.ca/product-detail/en/avx-corporation/F980J107MMAAXE/478-9836-1-ND/5957637"/>
+    <hyperlink ref="G17" r:id="rId14" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/DA2J10100L/DA2J10100LCT-ND/2184708"/>
+    <hyperlink ref="G34" r:id="rId15" display="http://www.digikey.ca/product-detail/en/molex-llc/1051620101/WM12823CT-ND/5823220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added change order to bom
</commit_message>
<xml_diff>
--- a/LPC Dev Board.xlsx
+++ b/LPC Dev Board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="184">
   <si>
     <t>Designator</t>
   </si>
@@ -458,9 +458,6 @@
     <t>150060GS75000 are $0.34</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
     <t xml:space="preserve">better choice </t>
   </si>
   <si>
@@ -549,6 +546,36 @@
   </si>
   <si>
     <t>SD card</t>
+  </si>
+  <si>
+    <t>74LVC1G04SE-7</t>
+  </si>
+  <si>
+    <t>Inverter for regulater enable</t>
+  </si>
+  <si>
+    <t>IRLML6244TRPBF</t>
+  </si>
+  <si>
+    <t>NMOS Power Switch</t>
+  </si>
+  <si>
+    <t>0/jumper</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF8062V</t>
+  </si>
+  <si>
+    <t>regulator bypass</t>
   </si>
 </sst>
 </file>
@@ -646,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,6 +691,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -979,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,13 +1040,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>145</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1037,11 +1065,14 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="G2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" t="s">
         <v>166</v>
-      </c>
-      <c r="H2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1054,6 +1085,9 @@
       <c r="E3" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1071,11 +1105,11 @@
       <c r="E4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F4">
-        <v>1.67</v>
+      <c r="F4" t="s">
+        <v>180</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1094,8 +1128,11 @@
       <c r="E5" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="F5" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="H5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1114,8 +1151,11 @@
       <c r="E6" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1134,9 +1174,12 @@
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1155,8 +1198,11 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G8" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1175,11 +1221,14 @@
       <c r="E9" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G9" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1198,11 +1247,14 @@
       <c r="E10" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="F10" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G10" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1221,14 +1273,14 @@
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11">
-        <v>3.12</v>
+      <c r="F11" t="s">
+        <v>180</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H11" t="s">
         <v>171</v>
-      </c>
-      <c r="H11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1247,11 +1299,11 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F12">
-        <v>0.56999999999999995</v>
+      <c r="F12" t="s">
+        <v>180</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1270,11 +1322,14 @@
       <c r="E13" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="F13" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G13" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1293,8 +1348,11 @@
       <c r="E14" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="F14" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1313,6 +1371,12 @@
       <c r="E15" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="F15" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H15" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1330,8 +1394,8 @@
       <c r="E16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F16">
-        <v>0.61</v>
+      <c r="F16" t="s">
+        <v>180</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>143</v>
@@ -1353,8 +1417,11 @@
       <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="F17" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G17" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1373,6 +1440,9 @@
       <c r="E18" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="F18" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -1390,6 +1460,9 @@
       <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="F19" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -1407,8 +1480,14 @@
       <c r="E20" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="F20" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="G20" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="H20" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1427,8 +1506,11 @@
       <c r="E21" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="F21" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G21" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1447,8 +1529,11 @@
       <c r="E22" s="2" t="s">
         <v>135</v>
       </c>
+      <c r="F22" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G22" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1467,8 +1552,11 @@
       <c r="E23" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="F23" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="H23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1487,8 +1575,11 @@
       <c r="E24" s="2" t="s">
         <v>137</v>
       </c>
+      <c r="F24" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="H24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1507,8 +1598,11 @@
       <c r="E25" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="F25" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="H25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1527,11 +1621,14 @@
       <c r="E26" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="F26" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G26" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1550,11 +1647,14 @@
       <c r="E27" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F27" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G27" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1573,8 +1673,14 @@
       <c r="E28" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="F28" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="H28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1593,8 +1699,11 @@
       <c r="E29" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="F29" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G29" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1613,6 +1722,9 @@
       <c r="E30" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="F30" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
@@ -1630,6 +1742,9 @@
       <c r="E31" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="F31" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -1647,6 +1762,9 @@
       <c r="E32" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="F32" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -1664,6 +1782,9 @@
       <c r="E33" s="2">
         <v>5017</v>
       </c>
+      <c r="F33" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -1681,11 +1802,14 @@
       <c r="E34" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="F34" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="G34" s="7">
         <v>1051620101</v>
       </c>
       <c r="H34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1704,6 +1828,9 @@
       <c r="E35" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="F35" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
@@ -1721,6 +1848,9 @@
       <c r="E36" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="F36" s="8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
@@ -1737,6 +1867,31 @@
       </c>
       <c r="E37" s="2" t="s">
         <v>123</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F38" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F39" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="H39" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1756,8 +1911,11 @@
     <hyperlink ref="G11" r:id="rId13" display="https://www.digikey.ca/product-detail/en/avx-corporation/F980J107MMAAXE/478-9836-1-ND/5957637"/>
     <hyperlink ref="G17" r:id="rId14" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/DA2J10100L/DA2J10100LCT-ND/2184708"/>
     <hyperlink ref="G34" r:id="rId15" display="http://www.digikey.ca/product-detail/en/molex-llc/1051620101/WM12823CT-ND/5823220"/>
+    <hyperlink ref="G38" r:id="rId16" display="http://www.digikey.ca/product-detail/en/diodes-incorporated/74LVC1G04SE-7/74LVC1G04SE-7DICT-ND/2330113"/>
+    <hyperlink ref="G39" r:id="rId17" display="http://www.digikey.ca/product-detail/en/infineon-technologies/IRLML6244TRPBF/IRLML6244TRPBFCT-ND/2393877"/>
+    <hyperlink ref="G28" r:id="rId18" display="http://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-3EKF8062V/P80.6KHCT-ND/198520"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished updating parts in schematic
</commit_message>
<xml_diff>
--- a/LPC Dev Board.xlsx
+++ b/LPC Dev Board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="182">
   <si>
     <t>Designator</t>
   </si>
@@ -455,9 +455,6 @@
     <t>Texas Instruments TPS7A4501DCQR</t>
   </si>
   <si>
-    <t>150060GS75000 are $0.34</t>
-  </si>
-  <si>
     <t xml:space="preserve">better choice </t>
   </si>
   <si>
@@ -564,9 +561,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>y</t>
@@ -1010,7 +1004,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,13 +1034,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1066,13 +1060,13 @@
         <v>8</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
         <v>165</v>
-      </c>
-      <c r="H2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1086,7 +1080,7 @@
         <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1106,10 +1100,10 @@
         <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1129,10 +1123,10 @@
         <v>61</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1152,10 +1146,10 @@
         <v>65</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1175,11 +1169,11 @@
         <v>12</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1199,10 +1193,10 @@
         <v>16</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1222,13 +1216,13 @@
         <v>128</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1248,13 +1242,13 @@
         <v>127</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1274,13 +1268,13 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" t="s">
         <v>170</v>
-      </c>
-      <c r="H11" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1300,10 +1294,10 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1323,13 +1317,13 @@
         <v>129</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1349,10 +1343,10 @@
         <v>130</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1372,10 +1366,10 @@
         <v>131</v>
       </c>
       <c r="F15" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" t="s">
         <v>181</v>
-      </c>
-      <c r="H15" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1395,11 +1389,9 @@
         <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>180</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>143</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1418,10 +1410,10 @@
         <v>43</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1441,7 +1433,7 @@
         <v>69</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1461,7 +1453,7 @@
         <v>53</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1481,13 +1473,13 @@
         <v>73</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1507,10 +1499,10 @@
         <v>134</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1530,10 +1522,10 @@
         <v>135</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1553,10 +1545,10 @@
         <v>136</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1576,10 +1568,10 @@
         <v>137</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1599,10 +1591,10 @@
         <v>138</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1622,13 +1614,13 @@
         <v>92</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1648,13 +1640,13 @@
         <v>139</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1674,13 +1666,13 @@
         <v>99</v>
       </c>
       <c r="F28" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="H28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1700,10 +1692,10 @@
         <v>103</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1723,7 +1715,7 @@
         <v>140</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1743,7 +1735,7 @@
         <v>141</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1763,7 +1755,7 @@
         <v>142</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1783,7 +1775,7 @@
         <v>5017</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1803,13 +1795,13 @@
         <v>133</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G34" s="7">
         <v>1051620101</v>
       </c>
       <c r="H34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1829,7 +1821,7 @@
         <v>116</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1849,7 +1841,7 @@
         <v>119</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1869,29 +1861,29 @@
         <v>123</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F38" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H38" t="s">
         <v>174</v>
-      </c>
-      <c r="H38" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F39" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G39" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H39" t="s">
         <v>176</v>
-      </c>
-      <c r="H39" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>